<commit_message>
groundwork for TF-IDF + NN
</commit_message>
<xml_diff>
--- a/Arun/Naive_Bayes/Comparison.xlsx
+++ b/Arun/Naive_Bayes/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Schoolwork\Y1.2 Frosh Spring\Summer\Project-C\Arun\Naive_Bayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6C9AF-2CC7-4DA0-A5FF-39123CA75EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB764AE-7768-4E0F-9FE9-1AE541712A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1221AA35-BCB8-4C74-B687-47C4736C9332}"/>
+    <workbookView xWindow="-10785" yWindow="6150" windowWidth="21600" windowHeight="11205" xr2:uid="{1221AA35-BCB8-4C74-B687-47C4736C9332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>15-0.1, Full Text</t>
+  </si>
+  <si>
+    <t>20-0.1, Full Text</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>20-0.05, Full Text</t>
+  </si>
+  <si>
+    <t>15-0.02, Full Text</t>
+  </si>
+  <si>
+    <t>25-0.02, Full Text</t>
+  </si>
+  <si>
+    <t>50-0.01, Full Text</t>
   </si>
 </sst>
 </file>
@@ -339,7 +357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A4B9DE6-4D65-4CB4-9E6D-4981E0207FAD}" type="CELLRANGE">
+                    <a:fld id="{788E9302-7320-45FD-9D39-912ADAC5D49D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -373,7 +391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3ABBF3F7-E325-40F3-9A77-D87ECC06D9B0}" type="CELLRANGE">
+                    <a:fld id="{8B141BDE-0112-41F7-BF22-31117B6A0908}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -407,7 +425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{431B8F52-BBF3-44DA-9151-F68DF7C15CAF}" type="CELLRANGE">
+                    <a:fld id="{FE68C80D-C216-499D-A37A-98706716B2D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -441,7 +459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5C03DBA-CDFB-45AC-BB47-8A2B16357E80}" type="CELLRANGE">
+                    <a:fld id="{8989F947-2B14-44A6-91F6-B3DB63A4F754}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -481,7 +499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7F59007-7C4C-4EAD-ADEF-1C0CB73F3DAC}" type="CELLRANGE">
+                    <a:fld id="{0ABF96E3-1430-4305-B21D-623DDAF4536B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -514,7 +532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFEEDDCE-1348-49B5-B84A-193546DD3DCB}" type="CELLRANGE">
+                    <a:fld id="{5F502716-5A23-4562-A5AC-5741E29664B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -548,7 +566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74CF729D-0CB1-4C70-9ED6-BBC5A30A22F2}" type="CELLRANGE">
+                    <a:fld id="{E9A4D0F2-C0FB-41C2-8F4B-CCF53AAEFC1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -588,7 +606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55CF4FAD-9B25-4280-946D-503F87648F9E}" type="CELLRANGE">
+                    <a:fld id="{2938424D-DC28-4095-8E66-FCAD31B2A551}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -627,7 +645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17861365-2148-4E24-AC5A-99B040CCC459}" type="CELLRANGE">
+                    <a:fld id="{A877A947-3F19-4898-91AC-3D30221000D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -666,7 +684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1096733A-FDC4-4FFD-B73B-1DC8F7049B03}" type="CELLRANGE">
+                    <a:fld id="{44FBAEFF-DBB0-44FE-A5A5-FC726C15463D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -705,7 +723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F397B7A0-CFE6-4172-9E5B-80508F26B812}" type="CELLRANGE">
+                    <a:fld id="{C13D9EAA-931F-4E5F-A8A2-6FAE01559054}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -733,12 +751,207 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7611928136964298E-2"/>
+                  <c:y val="0.20853696132911936"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6E7C769-5E87-4B18-ADC8-09B83B8F9D29}" type="CELLRANGE">
+                    <a:fld id="{EFEE0E75-FFB7-47A0-9E00-DB4B8DA93C3A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4698-439B-A6AF-2355F8768895}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.7810939348777405E-2"/>
+                  <c:y val="0.11990875276424363"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C0B860AD-784B-4725-AE0E-EEE7F6E9F798}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.1791038227596118E-2"/>
+                  <c:y val="8.6021496548261731E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D924D495-38DE-4ACE-BDAC-6AAA8A2EB247}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9552224773420341E-2"/>
+                  <c:y val="0.1981101132626634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BBA95F18-7975-491B-81D4-3ED157B544BC}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1890543833502748E-2"/>
+                  <c:y val="0.27891818577769706"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{107D0351-CE08-4C5B-8FD6-C5C533D94FB0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{37A75748-B834-4D68-A949-CAAB376BF559}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,7 +974,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-4698-439B-A6AF-2355F8768895}"/>
+                  <c16:uniqueId val="{00000006-A390-4896-B3CB-BDC18D5B49F3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -822,10 +1035,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:f>Sheet1!$E$2:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1.663</c:v>
                 </c:pt>
@@ -861,16 +1074,31 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.31798061826909796</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.36458022900763015</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.35258814961712343</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27294100086380163</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.33594723350244887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.35119127481962015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:f>Sheet1!$F$2:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.83599999999999997</c:v>
                 </c:pt>
@@ -906,6 +1134,21 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.67648695688420291</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.65972889161909132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65971257990172705</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69824085631250266</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6579212567586209</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64024083802081433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,9 +1157,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$B$2:$B$13</c15:f>
+                <c15:f>Sheet1!$B$2:$B$18</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="12"/>
+                  <c:ptCount val="17"/>
                   <c:pt idx="0">
                     <c:v>Old</c:v>
                   </c:pt>
@@ -952,6 +1195,21 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>15-0.1, Full Text</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20-0.1, Full Text</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>20-0.05, Full Text</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15-0.02, Full Text</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25-0.02, Full Text</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>50-0.01, Full Text</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1806,16 +2064,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2140,10 +2398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2ADD22-63B2-4186-B7AB-3D6251EEC8C5}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2415,7 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2179,8 +2437,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2196,8 +2457,12 @@
       <c r="G2">
         <v>2.4227205999999999</v>
       </c>
+      <c r="H2">
+        <f>E2+F2</f>
+        <v>2.4990000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -2207,8 +2472,12 @@
       <c r="F3">
         <v>0.81893997007389796</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H18" si="0">E3+F3</f>
+        <v>3.0564752284439778</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2221,8 +2490,12 @@
       <c r="F4">
         <v>0.96099999999999997</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.98199999999999998</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -2233,15 +2506,19 @@
         <v>2.2476603113357601</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:F13" si="0">C5/$G$2</f>
+        <f t="shared" ref="E5:F18" si="1">C5/$G$2</f>
         <v>2.1996967239331932E-2</v>
       </c>
       <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.9277422709559493</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.9277422709559493</v>
+        <v>0.94973923819528128</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -2252,15 +2529,19 @@
         <v>1.88565074780221</v>
       </c>
       <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.18585422474757182</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.77831952549634076</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.18585422474757182</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0.77831952549634076</v>
+        <v>0.96417375024391261</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -2271,15 +2552,19 @@
         <v>2.1350067720739001</v>
       </c>
       <c r="E7">
+        <f t="shared" si="1"/>
+        <v>3.5166579750653584E-2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.88124349628838761</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>3.5166579750653584E-2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.88124349628838761</v>
+        <v>0.91641007603904123</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -2290,15 +2575,19 @@
         <v>2.01510693410071</v>
       </c>
       <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.13140274642397931</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.83175374580985939</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.13140274642397931</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.83175374580985939</v>
+        <v>0.9631564922338387</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -2309,15 +2598,19 @@
         <v>1.8936263467804799</v>
       </c>
       <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.18119797088221029</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.7816115266368231</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>0.18119797088221029</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.7816115266368231</v>
+        <v>0.96280949751903333</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -2328,15 +2621,19 @@
         <v>1.89625973148816</v>
       </c>
       <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.18492890550808586</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.78269848016653676</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>0.18492890550808586</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.78269848016653676</v>
+        <v>0.96762738567462259</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -2347,15 +2644,19 @@
         <v>1.7336365497989901</v>
       </c>
       <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.26470951512920804</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.71557428033549975</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>0.26470951512920804</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0.71557428033549975</v>
+        <v>0.98028379546470779</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -2366,15 +2667,19 @@
         <v>1.72661299304111</v>
       </c>
       <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.2843858949188528</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.71267524329512455</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>0.2843858949188528</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.71267524329512455</v>
+        <v>0.99706113821397735</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -2385,12 +2690,131 @@
         <v>1.6389388860746701</v>
       </c>
       <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.31798061826909796</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.67648695688420291</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>0.31798061826909796</v>
-      </c>
-      <c r="F13">
+        <v>0.99446757515330086</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>0.88327603116950304</v>
+      </c>
+      <c r="D14">
+        <v>1.5983387761407399</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.36458022900763015</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.65972889161909132</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>0.67648695688420291</v>
+        <v>1.0243091206267214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>0.854222573393287</v>
+      </c>
+      <c r="D15">
+        <v>1.59829925740706</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.35258814961712343</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.65971257990172705</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.0123007295188504</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>0.66125978537734997</v>
+      </c>
+      <c r="D16">
+        <v>1.6916425063499401</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.27294100086380163</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.69824085631250266</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.97118185717630423</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>0.81390628311939295</v>
+      </c>
+      <c r="D17">
+        <v>1.5939593819269999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0.33594723350244887</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.6579212567586209</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.99386849026106971</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>0.85083833604575498</v>
+      </c>
+      <c r="D18">
+        <v>1.55112466723429</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.35119127481962015</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.64024083802081433</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.99143211284043442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging my wrapper code in Haimoshri's model and debugging my NN
</commit_message>
<xml_diff>
--- a/Arun/Naive_Bayes/Comparison.xlsx
+++ b/Arun/Naive_Bayes/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Schoolwork\Y1.2 Frosh Spring\Summer\Project-C\Arun\Naive_Bayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB764AE-7768-4E0F-9FE9-1AE541712A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D5E27-F273-4D7E-B572-57B210750672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10785" yWindow="6150" windowWidth="21600" windowHeight="11205" xr2:uid="{1221AA35-BCB8-4C74-B687-47C4736C9332}"/>
+    <workbookView xWindow="-10530" yWindow="6015" windowWidth="21600" windowHeight="11205" xr2:uid="{1221AA35-BCB8-4C74-B687-47C4736C9332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Model</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>50-0.01, Full Text</t>
+  </si>
+  <si>
+    <t>Lower</t>
   </si>
 </sst>
 </file>
@@ -240,9 +243,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Old</c:v>
                 </c:pt>
@@ -250,30 +253,33 @@
                   <c:v>New</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Lower</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Default, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Default, Title</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5-0.4, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>5-0.4, Title</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3-0.3, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>5-0.3, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>5-0.2, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10-0.4, Full Text</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>10-0.1, Full Text</c:v>
                 </c:pt>
               </c:strCache>
@@ -349,6 +355,30 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-E8B4-432F-9ED1-B87A4A36B68F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -357,7 +387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{788E9302-7320-45FD-9D39-912ADAC5D49D}" type="CELLRANGE">
+                    <a:fld id="{B7620590-563A-4A95-B193-A543F2FAB47F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -391,7 +421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B141BDE-0112-41F7-BF22-31117B6A0908}" type="CELLRANGE">
+                    <a:fld id="{66518DDC-2F76-4F39-BF1D-D05C8ABE9F3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -425,7 +455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE68C80D-C216-499D-A37A-98706716B2D3}" type="CELLRANGE">
+                    <a:fld id="{27C872FA-811E-45CF-851C-FE2FAD3BA0CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -459,7 +489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8989F947-2B14-44A6-91F6-B3DB63A4F754}" type="CELLRANGE">
+                    <a:fld id="{F14516EA-E601-4243-8A11-AC78CCF202C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -488,51 +518,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.14925370795570056"/>
-                  <c:y val="1.5640272099683904E-2"/>
-                </c:manualLayout>
-              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0ABF96E3-1430-4305-B21D-623DDAF4536B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-E8B4-432F-9ED1-B87A4A36B68F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{5F502716-5A23-4562-A5AC-5741E29664B2}" type="CELLRANGE">
+                    <a:fld id="{66E7E010-86FF-4414-BD20-373B4F7C3478}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -555,6 +546,45 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-E8B4-432F-9ED1-B87A4A36B68F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14925370795570056"/>
+                  <c:y val="1.5640272099683904E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0F90C931-9FDE-4DF9-B2DB-D835C80309A9}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-E8B4-432F-9ED1-B87A4A36B68F}"/>
                 </c:ext>
               </c:extLst>
@@ -566,7 +596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9A4D0F2-C0FB-41C2-8F4B-CCF53AAEFC1D}" type="CELLRANGE">
+                    <a:fld id="{FB4D08E0-ABAF-45DD-9284-93009AE2ACD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -595,363 +625,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.14925370795570053"/>
-                  <c:y val="-1.303356008306996E-2"/>
-                </c:manualLayout>
-              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2938424D-DC28-4095-8E66-FCAD31B2A551}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-E8B4-432F-9ED1-B87A4A36B68F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.15124375739510987"/>
-                  <c:y val="-4.1707392265823921E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{A877A947-3F19-4898-91AC-3D30221000D8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-E8B4-432F-9ED1-B87A4A36B68F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.20696514169857144"/>
-                  <c:y val="1.3033560083069912E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{44FBAEFF-DBB0-44FE-A5A5-FC726C15463D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-E8B4-432F-9ED1-B87A4A36B68F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.20298504281975269"/>
-                  <c:y val="4.692081629905176E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{C13D9EAA-931F-4E5F-A8A2-6FAE01559054}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-CB92-4D4E-BFC3-E20EFB9BCC71}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="11"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.7611928136964298E-2"/>
-                  <c:y val="0.20853696132911936"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{EFEE0E75-FFB7-47A0-9E00-DB4B8DA93C3A}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-4698-439B-A6AF-2355F8768895}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="12"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.7810939348777405E-2"/>
-                  <c:y val="0.11990875276424363"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{C0B860AD-784B-4725-AE0E-EEE7F6E9F798}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-A390-4896-B3CB-BDC18D5B49F3}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="13"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.1791038227596118E-2"/>
-                  <c:y val="8.6021496548261731E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{D924D495-38DE-4ACE-BDAC-6AAA8A2EB247}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-A390-4896-B3CB-BDC18D5B49F3}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="14"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.9552224773420341E-2"/>
-                  <c:y val="0.1981101132626634"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{BBA95F18-7975-491B-81D4-3ED157B544BC}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-A390-4896-B3CB-BDC18D5B49F3}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="15"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="2.1890543833502748E-2"/>
-                  <c:y val="0.27891818577769706"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{107D0351-CE08-4C5B-8FD6-C5C533D94FB0}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-A390-4896-B3CB-BDC18D5B49F3}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="16"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{37A75748-B834-4D68-A949-CAAB376BF559}" type="CELLRANGE">
+                    <a:fld id="{C628E4BA-325A-4D56-8FBE-1060736EAB87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -974,7 +653,420 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-E8B4-432F-9ED1-B87A4A36B68F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14925370795570053"/>
+                  <c:y val="-1.303356008306996E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2E98D937-0ACC-4167-8B5E-FA7CB270A1AA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E8B4-432F-9ED1-B87A4A36B68F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15124375739510987"/>
+                  <c:y val="-4.1707392265823921E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0611B245-E7F2-4980-B08E-7B17BBE5349F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-E8B4-432F-9ED1-B87A4A36B68F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.20696514169857144"/>
+                  <c:y val="1.3033560083069912E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E3EEBA7C-46C9-4CA6-966F-F45A3F0765AA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-CB92-4D4E-BFC3-E20EFB9BCC71}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.20298504281975269"/>
+                  <c:y val="4.692081629905176E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1950C5E0-19A7-45F5-A5F4-036A19603916}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4698-439B-A6AF-2355F8768895}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7611928136964298E-2"/>
+                  <c:y val="0.20853696132911936"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D933C226-DA82-4268-B0CF-921702E9B068}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.7810939348777405E-2"/>
+                  <c:y val="0.11990875276424363"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3EB44BC5-F108-4A67-A40C-34971E5C1F9B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.1791038227596118E-2"/>
+                  <c:y val="8.6021496548261731E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{320DE886-F981-46B8-9BFA-7BEE552E4170}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9552224773420341E-2"/>
+                  <c:y val="0.1981101132626634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0658D064-B2A5-46F7-B1B7-8AFA30A44473}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1890543833502748E-2"/>
+                  <c:y val="0.27891818577769706"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{16262D1F-9D2B-46F2-8FC2-98423C750AE7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-A390-4896-B3CB-BDC18D5B49F3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B4BCD502-F9DD-40E9-AAF7-A325A3966916}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-8C4D-470A-971F-004B73633EC5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-DDE3-4A9A-A5F1-58AD33809149}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1035,10 +1127,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$18</c:f>
+              <c:f>Sheet1!$E$2:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1.663</c:v>
                 </c:pt>
@@ -1046,59 +1138,65 @@
                   <c:v>2.2375352583700798</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2.5006976602967099</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.1996967239331932E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.18585422474757182</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3.5166579750653584E-2</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.13140274642397931</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.18119797088221029</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.18492890550808586</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.26470951512920804</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.2843858949188528</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.31798061826909796</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.36458022900763015</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.35258814961712343</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.27294100086380163</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.33594723350244887</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.35119127481962015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61541440419473881</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$18</c:f>
+              <c:f>Sheet1!$F$2:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.83599999999999997</c:v>
                 </c:pt>
@@ -1106,49 +1204,55 @@
                   <c:v>0.81893997007389796</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.76700659579811203</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.96099999999999997</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.9277422709559493</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.77831952549634076</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.88124349628838761</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.83175374580985939</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.7816115266368231</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.78269848016653676</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.71557428033549975</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.71267524329512455</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.67648695688420291</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.65972889161909132</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.65971257990172705</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.69824085631250266</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.6579212567586209</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.64024083802081433</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0491889382550759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,9 +1261,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$B$2:$B$18</c15:f>
+                <c15:f>Sheet1!$B$2:$B$19</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="17"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>Old</c:v>
                   </c:pt>
@@ -1167,48 +1271,51 @@
                     <c:v>New</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>Lower</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>Default, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>Default, Title</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>5-0.4, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>5-0.4, Title</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>3-0.3, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>5-0.3, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>5-0.2, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>10-0.4, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>10-0.1, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>15-0.1, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>20-0.1, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>20-0.05, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>15-0.02, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>25-0.02, Full Text</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>50-0.01, Full Text</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -2065,15 +2172,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2398,11 +2505,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2ADD22-63B2-4186-B7AB-3D6251EEC8C5}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2473,348 +2578,382 @@
         <v>0.81893997007389796</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H18" si="0">E3+F3</f>
+        <f t="shared" ref="H3:H20" si="0">E3+F3</f>
         <v>3.0564752284439778</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>2.5006976602967099</v>
+      </c>
+      <c r="F4">
+        <v>0.76700659579811203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>0.96099999999999997</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>0.98199999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>5.3292505668254601E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.2476603113357601</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5:F18" si="1">C5/$G$2</f>
-        <v>2.1996967239331932E-2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0.9277422709559493</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>0.94973923819528128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>0.45027285889297203</v>
+        <v>5.3292505668254601E-2</v>
       </c>
       <c r="D6">
-        <v>1.88565074780221</v>
+        <v>2.2476603113357601</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0.18585422474757182</v>
+        <f t="shared" ref="E6:F20" si="1">C6/$G$2</f>
+        <v>2.1996967239331932E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>0.77831952549634076</v>
+        <v>0.9277422709559493</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.96417375024391261</v>
+        <v>0.94973923819528128</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>8.5198797193451303E-2</v>
+        <v>0.45027285889297203</v>
       </c>
       <c r="D7">
-        <v>2.1350067720739001</v>
+        <v>1.88565074780221</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>3.5166579750653584E-2</v>
+        <v>0.18585422474757182</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>0.88124349628838761</v>
+        <v>0.77831952549634076</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.91641007603904123</v>
+        <v>0.96417375024391261</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>0.31835214065795098</v>
+        <v>8.5198797193451303E-2</v>
       </c>
       <c r="D8">
-        <v>2.01510693410071</v>
+        <v>2.1350067720739001</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0.13140274642397931</v>
+        <v>3.5166579750653584E-2</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>0.83175374580985939</v>
+        <v>0.88124349628838761</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.9631564922338387</v>
+        <v>0.91641007603904123</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0.43899205673453101</v>
+        <v>0.31835214065795098</v>
       </c>
       <c r="D9">
-        <v>1.8936263467804799</v>
+        <v>2.01510693410071</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0.18119797088221029</v>
+        <v>0.13140274642397931</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0.7816115266368231</v>
+        <v>0.83175374580985939</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0.96280949751903333</v>
+        <v>0.9631564922338387</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>0.44803106890989303</v>
+        <v>0.43899205673453101</v>
       </c>
       <c r="D10">
-        <v>1.89625973148816</v>
+        <v>1.8936263467804799</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.18492890550808586</v>
+        <v>0.18119797088221029</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>0.78269848016653676</v>
+        <v>0.7816115266368231</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0.96762738567462259</v>
+        <v>0.96280949751903333</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>0.64131719531954401</v>
+        <v>0.44803106890989303</v>
       </c>
       <c r="D11">
-        <v>1.7336365497989901</v>
+        <v>1.89625973148816</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0.26470951512920804</v>
+        <v>0.18492890550808586</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>0.71557428033549975</v>
+        <v>0.78269848016653676</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>0.98028379546470779</v>
+        <v>0.96762738567462259</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>0.68898756596933997</v>
+        <v>0.64131719531954401</v>
       </c>
       <c r="D12">
-        <v>1.72661299304111</v>
+        <v>1.7336365497989901</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0.2843858949188528</v>
+        <v>0.26470951512920804</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.71267524329512455</v>
+        <v>0.71557428033549975</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>0.99706113821397735</v>
+        <v>0.98028379546470779</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>0.77037819428127996</v>
+        <v>0.68898756596933997</v>
       </c>
       <c r="D13">
-        <v>1.6389388860746701</v>
+        <v>1.72661299304111</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0.31798061826909796</v>
+        <v>0.2843858949188528</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0.67648695688420291</v>
+        <v>0.71267524329512455</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0.99446757515330086</v>
+        <v>0.99706113821397735</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>0.88327603116950304</v>
+        <v>0.77037819428127996</v>
       </c>
       <c r="D14">
-        <v>1.5983387761407399</v>
+        <v>1.6389388860746701</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>0.36458022900763015</v>
+        <v>0.31798061826909796</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0.65972889161909132</v>
+        <v>0.67648695688420291</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1.0243091206267214</v>
+        <v>0.99446757515330086</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>0.854222573393287</v>
+        <v>0.88327603116950304</v>
       </c>
       <c r="D15">
-        <v>1.59829925740706</v>
+        <v>1.5983387761407399</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0.35258814961712343</v>
+        <v>0.36458022900763015</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.65971257990172705</v>
+        <v>0.65972889161909132</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1.0123007295188504</v>
+        <v>1.0243091206267214</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16">
-        <v>0.66125978537734997</v>
+        <v>0.854222573393287</v>
       </c>
       <c r="D16">
-        <v>1.6916425063499401</v>
+        <v>1.59829925740706</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>0.27294100086380163</v>
+        <v>0.35258814961712343</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0.69824085631250266</v>
+        <v>0.65971257990172705</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0.97118185717630423</v>
+        <v>1.0123007295188504</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>0.81390628311939295</v>
+        <v>0.66125978537734997</v>
       </c>
       <c r="D17">
-        <v>1.5939593819269999</v>
+        <v>1.6916425063499401</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>0.33594723350244887</v>
+        <v>0.27294100086380163</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0.6579212567586209</v>
+        <v>0.69824085631250266</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>0.99386849026106971</v>
+        <v>0.97118185717630423</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18">
-        <v>0.85083833604575498</v>
+        <v>0.81390628311939295</v>
       </c>
       <c r="D18">
-        <v>1.55112466723429</v>
+        <v>1.5939593819269999</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>0.35119127481962015</v>
+        <v>0.33594723350244887</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0.64024083802081433</v>
+        <v>0.6579212567586209</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
+        <v>0.99386849026106971</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>0.85083833604575498</v>
+      </c>
+      <c r="D19">
+        <v>1.55112466723429</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.35119127481962015</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.64024083802081433</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
         <v>0.99143211284043442</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>1.49097715457932</v>
+      </c>
+      <c r="D20">
+        <v>2.5418916540027001</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.61541440419473881</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>1.0491889382550759</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1.6646033424498148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>